<commit_message>
Add bias and activation after convolution
</commit_message>
<xml_diff>
--- a/docs/Accum_pipe.xlsx
+++ b/docs/Accum_pipe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE98173-54BB-4CFD-BC16-CBA86B4A4678}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF797C32-CE9C-44C0-977C-2A96A39E7E1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" xr2:uid="{DEEA8246-510E-4920-BF6B-C93439445055}"/>
   </bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
-  <si>
-    <t>√</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>1~64</t>
   </si>
@@ -47,10 +44,25 @@
     <t>129~160</t>
   </si>
   <si>
-    <t>Final One</t>
+    <t>161-168</t>
   </si>
   <si>
-    <t>161-168</t>
+    <t>Final 6</t>
+  </si>
+  <si>
+    <t>1+2</t>
+  </si>
+  <si>
+    <t>3+4</t>
+  </si>
+  <si>
+    <t>1+2+6</t>
+  </si>
+  <si>
+    <t>3+4+5</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -66,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -289,7 +307,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -613,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF937D4-35C6-4452-B26A-AD87E39E9FA9}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,17 +643,21 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
+      <c r="G1" s="13">
+        <v>1</v>
+      </c>
+      <c r="H1" s="33">
+        <v>3</v>
+      </c>
+      <c r="I1" s="34">
+        <v>5</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>10</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -649,11 +671,13 @@
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="32" t="s">
-        <v>0</v>
+      <c r="G2" s="32">
+        <v>2</v>
       </c>
       <c r="H2" s="17"/>
-      <c r="I2" s="38"/>
+      <c r="I2" s="38" t="s">
+        <v>7</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -669,7 +693,9 @@
       <c r="F3" s="21"/>
       <c r="G3" s="19"/>
       <c r="H3" s="26"/>
-      <c r="I3" s="36"/>
+      <c r="I3" s="38" t="s">
+        <v>8</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -683,8 +709,8 @@
       <c r="E4" s="16"/>
       <c r="F4" s="30"/>
       <c r="G4" s="27"/>
-      <c r="H4" s="31" t="s">
-        <v>0</v>
+      <c r="H4" s="31">
+        <v>4</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -700,7 +726,7 @@
       <c r="F5" s="19"/>
       <c r="G5" s="17"/>
       <c r="H5" s="38" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -968,19 +994,19 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B34" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="D34" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="F34" s="14" t="s">
         <v>4</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>6</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14">

</xml_diff>

<commit_message>
changes for thesis writing
</commit_message>
<xml_diff>
--- a/docs/Accum_pipe.xlsx
+++ b/docs/Accum_pipe.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palad\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF797C32-CE9C-44C0-977C-2A96A39E7E1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E2EE8-B058-48B9-AA18-A463D8BBA6FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" xr2:uid="{DEEA8246-510E-4920-BF6B-C93439445055}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DEEA8246-510E-4920-BF6B-C93439445055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>1~64</t>
   </si>
@@ -47,9 +50,6 @@
     <t>161-168</t>
   </si>
   <si>
-    <t>Final 6</t>
-  </si>
-  <si>
     <t>1+2</t>
   </si>
   <si>
@@ -64,17 +64,42 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>Cycle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accumulator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -218,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -231,88 +256,95 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,7 +365,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,284 +661,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF937D4-35C6-4452-B26A-AD87E39E9FA9}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.9140625" customWidth="1"/>
+    <col min="8" max="8" width="4.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.9140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13">
+    <row r="1" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16">
         <v>1</v>
       </c>
-      <c r="H1" s="33">
+      <c r="H1" s="17">
         <v>3</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="18">
         <v>5</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>10</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="36"/>
-    </row>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="32">
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="41"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22">
         <v>2</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="38" t="s">
-        <v>7</v>
-      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="11"/>
-      <c r="R2" s="36"/>
-    </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="19"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="41"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="26"/>
-      <c r="I3" s="38" t="s">
-        <v>8</v>
-      </c>
+      <c r="I3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="31">
+    <row r="4" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29">
         <v>4</v>
       </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="38" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="36"/>
-    </row>
-    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="35" t="s">
-        <v>5</v>
-      </c>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="41"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33">
+        <v>6</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="7"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="18"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="8"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="27"/>
+    <row r="8" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="41"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="26"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="8"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="23"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="8"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="25"/>
+    <row r="10" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="41"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="M10" s="2"/>
       <c r="N10" s="3"/>
       <c r="O10" s="9"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="18"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
       <c r="M11" s="2"/>
       <c r="N11" s="7"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="18"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
       <c r="M12" s="2"/>
       <c r="N12" s="8"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="18"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
       <c r="M13" s="2"/>
       <c r="N13" s="8"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="18"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="M14" s="2"/>
       <c r="N14" s="8"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="18"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
       <c r="M15" s="2"/>
       <c r="N15" s="8"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="27"/>
+    <row r="16" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="41"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="26"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
       <c r="M16" s="2"/>
       <c r="N16" s="8"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="12"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="23"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
       <c r="M17" s="2"/>
       <c r="N17" s="8"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="15"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="24"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
       <c r="M18" s="2"/>
       <c r="N18" s="8"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" s="15"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="24"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
       <c r="M19" s="2"/>
       <c r="N19" s="8"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="15"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
+    <row r="20" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="41"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
       <c r="M20" s="3"/>
       <c r="N20" s="9"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="18"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="41"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="M22">
         <v>40</v>
       </c>
@@ -929,125 +1087,204 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B24" s="15"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="18"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="18"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="18"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="18"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B30" s="15"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="18"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B31" s="15"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="18"/>
-    </row>
-    <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="16"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="27"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="41"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="41"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="26"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B33" s="14"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="37" t="s">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C33" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D33" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E33" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F33" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14">
+      <c r="G33" s="39"/>
+      <c r="H33" s="39">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14">
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="39">
         <v>1</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C34" s="39">
         <v>2</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D34" s="39">
         <v>3</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E34" s="39">
         <v>4</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F34" s="39">
         <v>5</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G34" s="39">
         <v>6</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H34" s="39">
         <v>7</v>
       </c>
-      <c r="I35" s="14">
+      <c r="I34" s="39">
         <v>8</v>
       </c>
-      <c r="J35" s="14">
+      <c r="J34" s="39">
         <v>9</v>
       </c>
-      <c r="K35" s="14">
+      <c r="K34" s="39">
         <v>10</v>
       </c>
-      <c r="L35" s="14"/>
+      <c r="L34" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A32"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Some changes related to thesis
</commit_message>
<xml_diff>
--- a/docs/Accum_pipe.xlsx
+++ b/docs/Accum_pipe.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shish\source\repos\FusionAccel\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palad\source\repos\FusionAccel\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF797C32-CE9C-44C0-977C-2A96A39E7E1D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E2EE8-B058-48B9-AA18-A463D8BBA6FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6910" xr2:uid="{DEEA8246-510E-4920-BF6B-C93439445055}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{DEEA8246-510E-4920-BF6B-C93439445055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$34</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>1~64</t>
   </si>
@@ -47,9 +50,6 @@
     <t>161-168</t>
   </si>
   <si>
-    <t>Final 6</t>
-  </si>
-  <si>
     <t>1+2</t>
   </si>
   <si>
@@ -64,17 +64,42 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>Cycle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Accumulator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -218,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -231,88 +256,95 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -333,7 +365,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,284 +661,410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF937D4-35C6-4452-B26A-AD87E39E9FA9}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.9140625" customWidth="1"/>
+    <col min="8" max="8" width="4.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.9140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.08203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13">
+    <row r="1" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16">
         <v>1</v>
       </c>
-      <c r="H1" s="33">
+      <c r="H1" s="17">
         <v>3</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="18">
         <v>5</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>10</v>
       </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="36"/>
-    </row>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="32">
+      <c r="R1" s="13"/>
+    </row>
+    <row r="2" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="41"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22">
         <v>2</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="38" t="s">
-        <v>7</v>
-      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="11"/>
-      <c r="R2" s="36"/>
-    </row>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="19"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="41"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="26"/>
-      <c r="I3" s="38" t="s">
-        <v>8</v>
-      </c>
+      <c r="I3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="31">
+    <row r="4" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29">
         <v>4</v>
       </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="38" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="41"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="36"/>
-    </row>
-    <row r="6" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="35" t="s">
-        <v>5</v>
-      </c>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="41"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33">
+        <v>6</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="7"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="18"/>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="8"/>
       <c r="P7" s="5"/>
     </row>
-    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="27"/>
+    <row r="8" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="41"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="26"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="8"/>
       <c r="P8" s="5"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="23"/>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="8"/>
       <c r="P9" s="5"/>
     </row>
-    <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="25"/>
+    <row r="10" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="41"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="M10" s="2"/>
       <c r="N10" s="3"/>
       <c r="O10" s="9"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="18"/>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
       <c r="M11" s="2"/>
       <c r="N11" s="7"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="18"/>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
       <c r="M12" s="2"/>
       <c r="N12" s="8"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="18"/>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
       <c r="M13" s="2"/>
       <c r="N13" s="8"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="18"/>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
       <c r="M14" s="2"/>
       <c r="N14" s="8"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="18"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
       <c r="M15" s="2"/>
       <c r="N15" s="8"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="27"/>
+    <row r="16" spans="1:18" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="41"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
       <c r="F16" s="26"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
       <c r="M16" s="2"/>
       <c r="N16" s="8"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B17" s="12"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="23"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="41"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
       <c r="M17" s="2"/>
       <c r="N17" s="8"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="15"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="24"/>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="41"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
       <c r="M18" s="2"/>
       <c r="N18" s="8"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B19" s="15"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="24"/>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="41"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
       <c r="M19" s="2"/>
       <c r="N19" s="8"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="15"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="25"/>
+    <row r="20" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="41"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
       <c r="M20" s="3"/>
       <c r="N20" s="9"/>
       <c r="O20" s="6"/>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B21" s="15"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="18"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="18"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="41"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="M22">
         <v>40</v>
       </c>
@@ -929,125 +1087,204 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B23" s="15"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="18"/>
-    </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B24" s="15"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="18"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B26" s="15"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="18"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="15"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="15"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="18"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="18"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B30" s="15"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="18"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B31" s="15"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="18"/>
-    </row>
-    <row r="32" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="16"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="27"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="41"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="41"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="41"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="41"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27" s="41"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" s="41"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="41"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" s="41"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31" s="41"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:19" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="41"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="26"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B33" s="14"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="37" t="s">
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C33" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D33" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E33" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F33" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14">
+      <c r="G33" s="39"/>
+      <c r="H33" s="39">
         <v>169</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14">
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="39">
         <v>1</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C34" s="39">
         <v>2</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D34" s="39">
         <v>3</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E34" s="39">
         <v>4</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F34" s="39">
         <v>5</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G34" s="39">
         <v>6</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H34" s="39">
         <v>7</v>
       </c>
-      <c r="I35" s="14">
+      <c r="I34" s="39">
         <v>8</v>
       </c>
-      <c r="J35" s="14">
+      <c r="J34" s="39">
         <v>9</v>
       </c>
-      <c r="K35" s="14">
+      <c r="K34" s="39">
         <v>10</v>
       </c>
-      <c r="L35" s="14"/>
+      <c r="L34" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A32"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>